<commit_message>
Version finale Fiche de paie Anka avec l'ajout de Autre allocation
</commit_message>
<xml_diff>
--- a/ModèleFiche/FICHE DE PAIE 2024.xlsx
+++ b/ModèleFiche/FICHE DE PAIE 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CE PC\Desktop\FicheDePaie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CE PC\Desktop\FicheDePaie\ModèleFiche\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D9F5D-8828-4DCE-8539-3AD0C4EADE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6651424C-E19B-41D9-AEA9-DE10DD681A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>ANKA Madagascar SARL</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>"lu et approuvé"</t>
+  </si>
+  <si>
+    <t>Autre allocation</t>
   </si>
 </sst>
 </file>
@@ -950,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2098,7 +2101,7 @@
       <c r="C49" s="6"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22">
-        <f>+E43-D51</f>
+        <f>+E43-D52</f>
         <v>0</v>
       </c>
       <c r="F49" s="38"/>
@@ -2125,13 +2128,10 @@
     <row r="51" spans="1:9" ht="15.75" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="27" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C51" s="6"/>
-      <c r="D51" s="48">
-        <f>D48-D50</f>
-        <v>0</v>
-      </c>
+      <c r="D51" s="46"/>
       <c r="E51" s="22"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -2140,10 +2140,15 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1">
       <c r="A52" s="3"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="52"/>
+      <c r="B52" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="48">
+        <f>D48-D50</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="22"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2151,37 +2156,37 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1">
       <c r="A53" s="3"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="54">
-        <f>ROUNDDOWN(E49,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="55"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="42"/>
-    </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1">
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="3"/>
+      <c r="D54" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="54">
+        <f>ROUNDDOWN(E49,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="55"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9" ht="15.75" customHeight="1">
+      <c r="H54" s="38"/>
+      <c r="I54" s="42"/>
+    </row>
+    <row r="55" spans="1:9" ht="13.5" customHeight="1">
       <c r="A55" s="3"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="58"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="57"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -2189,10 +2194,10 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1">
       <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+      <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="E56" s="58"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -2200,31 +2205,42 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1">
       <c r="A57" s="3"/>
-      <c r="B57" s="59" t="s">
-        <v>34</v>
-      </c>
+      <c r="B57" s="3"/>
       <c r="C57" s="6"/>
-      <c r="D57" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="E57" s="59"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:9" ht="15.75" customHeight="1">
       <c r="A58" s="3"/>
-      <c r="B58" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="68"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
+      <c r="B58" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="59"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" ht="15">
+      <c r="A59" s="3"/>
+      <c r="B59" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="68"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2232,7 +2248,7 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>